<commit_message>
18.04, started to make docs
</commit_message>
<xml_diff>
--- a/ExcelDogovor/ExcelDefs/lists/IT_project.xlsx
+++ b/ExcelDogovor/ExcelDefs/lists/IT_project.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Лист6" sheetId="7" r:id="rId7"/>
     <sheet name="Лист7" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
   <si>
     <t>GROUP_NAME:</t>
   </si>
@@ -67,18 +67,6 @@
     <t>NAME:</t>
   </si>
   <si>
-    <t>Zolotarev</t>
-  </si>
-  <si>
-    <t>Maxim</t>
-  </si>
-  <si>
-    <t>Vasil'evich</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>GENDER:</t>
   </si>
   <si>
@@ -88,9 +76,6 @@
     <t>SCHOOL:</t>
   </si>
   <si>
-    <t>Liceum №1 im. A. S. Pushkina</t>
-  </si>
-  <si>
     <t>SCHOOL_SCHEDULE:</t>
   </si>
   <si>
@@ -106,24 +91,6 @@
     <t>CERTIFICATE_NUM:</t>
   </si>
   <si>
-    <t>XXXXXXXXX</t>
-  </si>
-  <si>
-    <t>Vasily</t>
-  </si>
-  <si>
-    <t>Borisovich</t>
-  </si>
-  <si>
-    <t>Zolotareva</t>
-  </si>
-  <si>
-    <t>Elena</t>
-  </si>
-  <si>
-    <t>Nikolaevna</t>
-  </si>
-  <si>
     <t>FIO_Parent1:</t>
   </si>
   <si>
@@ -149,12 +116,93 @@
   </si>
   <si>
     <t>PAYMENT_COST:</t>
+  </si>
+  <si>
+    <t>М</t>
+  </si>
+  <si>
+    <t>Золотарев Максим Васильевич</t>
+  </si>
+  <si>
+    <t>Золотарева Елена Николаевна</t>
+  </si>
+  <si>
+    <t>FIO_Parent:</t>
+  </si>
+  <si>
+    <t>МАОУ Лицей №1 им. А. С. Пушкина</t>
+  </si>
+  <si>
+    <t>10 Г</t>
+  </si>
+  <si>
+    <t>Parent_MOBILE_NUM:</t>
+  </si>
+  <si>
+    <t>STUD_PASSPORT_NUM:</t>
+  </si>
+  <si>
+    <t>STUD_PASSPORT_PLACE:</t>
+  </si>
+  <si>
+    <t>Parent_PASSPORT_NUM:</t>
+  </si>
+  <si>
+    <t>Parent_PASSPORT_PLACE:</t>
+  </si>
+  <si>
+    <t>CERT_NUM</t>
+  </si>
+  <si>
+    <t>STUD_Serial</t>
+  </si>
+  <si>
+    <t>PAR_Serial</t>
+  </si>
+  <si>
+    <t>PAR_Num</t>
+  </si>
+  <si>
+    <t>STUD_Num</t>
+  </si>
+  <si>
+    <t>FIO_Student:</t>
+  </si>
+  <si>
+    <t>CLASS:</t>
+  </si>
+  <si>
+    <t>DATE_START:</t>
+  </si>
+  <si>
+    <t>DATE_END:</t>
+  </si>
+  <si>
+    <t>HOURS:</t>
+  </si>
+  <si>
+    <t>УФМС по Кировскому району</t>
+  </si>
+  <si>
+    <t>УФМС по Советскому району</t>
+  </si>
+  <si>
+    <t>LIVING_ADRESS:</t>
+  </si>
+  <si>
+    <t>ул. Учебная, 228, кв. 63</t>
+  </si>
+  <si>
+    <t>03.09.2019</t>
+  </si>
+  <si>
+    <t>30.12.2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -192,11 +240,16 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -477,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,54 +551,79 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.75694444444444453</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.75694444444444453</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
         <v>0.81944444444444453</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -564,23 +642,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
+      <c r="A3" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>18</v>
+      <c r="A4" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C4">
         <f ca="1">DATEDIF(B4,TODAY(),"Y")</f>
@@ -588,83 +666,83 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>38</v>
+      <c r="A18" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>37</v>
+      <c r="A19" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>39</v>
+      <c r="A20" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>40</v>
+      <c r="A21" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -674,178 +752,179 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="4" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="3">
         <v>777777</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>37772</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <f ca="1">DATEDIF(B4,TODAY(),"Y")</f>
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -858,7 +937,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,23 +947,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
+      <c r="A3" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>18</v>
+      <c r="A4" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C4">
         <f ca="1">DATEDIF(B4,TODAY(),"Y")</f>
@@ -892,83 +971,83 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>38</v>
+      <c r="A18" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>37</v>
+      <c r="A19" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>39</v>
+      <c r="A20" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>40</v>
+      <c r="A21" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -991,23 +1070,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
+      <c r="A3" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>18</v>
+      <c r="A4" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C4">
         <f ca="1">DATEDIF(B4,TODAY(),"Y")</f>
@@ -1015,83 +1094,83 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>38</v>
+      <c r="A18" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>37</v>
+      <c r="A19" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>39</v>
+      <c r="A20" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>40</v>
+      <c r="A21" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>